<commit_message>
Update [Raw to Processed]
</commit_message>
<xml_diff>
--- a/schema_dict/schema_dict.xlsx
+++ b/schema_dict/schema_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2303c794d4905f1/Escritorio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_B3EF674BC126D8F078DEDED8D9E05D15841C0DD9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F221F473-FD93-4B40-8BFA-F562C40E1727}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="11_B3EF674BC126D8F078DEDED8D9E05D15841C0DD9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62CCFE9A-5A1F-46B1-B9B4-4EA315DAE401}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="195">
   <si>
     <t>Organizacion</t>
   </si>
@@ -879,7 +879,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1081,9 +1081,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1328,7 +1325,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+      <selection pane="bottomLeft" activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8227,7 +8224,9 @@
       <c r="C73" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="D73" s="76"/>
+      <c r="D73" s="49" t="s">
+        <v>194</v>
+      </c>
       <c r="E73" s="75" t="s">
         <v>68</v>
       </c>
@@ -8317,7 +8316,9 @@
       <c r="A74" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="42"/>
+      <c r="B74" s="49" t="s">
+        <v>194</v>
+      </c>
       <c r="C74" s="49" t="s">
         <v>194</v>
       </c>
@@ -8423,7 +8424,9 @@
       <c r="G75" s="75" t="s">
         <v>176</v>
       </c>
-      <c r="H75" s="75"/>
+      <c r="H75" s="49" t="s">
+        <v>194</v>
+      </c>
       <c r="I75" s="16"/>
       <c r="J75" s="55" t="s">
         <v>185</v>
@@ -8507,9 +8510,13 @@
       <c r="E76" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="F76" s="82"/>
-      <c r="G76" s="91"/>
-      <c r="H76" s="91"/>
+      <c r="F76" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="G76" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="H76" s="90"/>
       <c r="I76" s="16"/>
       <c r="J76" s="55" t="s">
         <v>185</v>
@@ -8670,7 +8677,9 @@
       <c r="BZ77" s="13"/>
     </row>
     <row r="78" spans="1:78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
+      <c r="A78" s="49" t="s">
+        <v>194</v>
+      </c>
       <c r="B78" s="42"/>
       <c r="C78" s="49"/>
       <c r="D78" s="49"/>
@@ -8758,12 +8767,16 @@
       <c r="B79" s="42"/>
       <c r="C79" s="49"/>
       <c r="D79" s="49"/>
-      <c r="E79" s="49"/>
+      <c r="E79" s="49" t="s">
+        <v>194</v>
+      </c>
       <c r="F79" s="19"/>
       <c r="G79" s="49"/>
       <c r="H79" s="49"/>
       <c r="I79" s="16"/>
-      <c r="J79" s="16"/>
+      <c r="J79" s="16" t="s">
+        <v>185</v>
+      </c>
       <c r="K79" s="14"/>
       <c r="L79" s="14"/>
       <c r="M79" s="13"/>
@@ -8918,10 +8931,10 @@
       <c r="B81" s="42"/>
       <c r="C81" s="49"/>
       <c r="D81" s="49"/>
-      <c r="E81" s="84"/>
+      <c r="E81" s="83"/>
       <c r="F81" s="70"/>
-      <c r="G81" s="84"/>
-      <c r="H81" s="84"/>
+      <c r="G81" s="83"/>
+      <c r="H81" s="83"/>
       <c r="I81" s="33"/>
       <c r="J81" s="33"/>
       <c r="K81" s="31"/>
@@ -9078,71 +9091,71 @@
       <c r="B83" s="42"/>
       <c r="C83" s="49"/>
       <c r="D83" s="49"/>
-      <c r="E83" s="83"/>
+      <c r="E83" s="82"/>
       <c r="F83" s="72"/>
-      <c r="G83" s="92"/>
-      <c r="H83" s="92"/>
-      <c r="I83" s="85"/>
-      <c r="J83" s="85"/>
-      <c r="K83" s="86"/>
-      <c r="L83" s="86"/>
-      <c r="M83" s="87"/>
-      <c r="N83" s="87"/>
-      <c r="O83" s="87"/>
-      <c r="P83" s="87"/>
-      <c r="Q83" s="87"/>
-      <c r="R83" s="87"/>
-      <c r="S83" s="87"/>
-      <c r="T83" s="88"/>
-      <c r="U83" s="89"/>
-      <c r="V83" s="89"/>
-      <c r="W83" s="90"/>
-      <c r="X83" s="90"/>
-      <c r="Y83" s="87"/>
-      <c r="Z83" s="87"/>
-      <c r="AA83" s="87"/>
-      <c r="AB83" s="86"/>
-      <c r="AC83" s="86"/>
-      <c r="AD83" s="86"/>
-      <c r="AE83" s="86"/>
-      <c r="AF83" s="86"/>
-      <c r="AG83" s="86"/>
-      <c r="AH83" s="86"/>
-      <c r="AI83" s="86"/>
-      <c r="AJ83" s="86"/>
-      <c r="AK83" s="86"/>
-      <c r="AL83" s="86"/>
-      <c r="AM83" s="86"/>
-      <c r="AN83" s="86"/>
-      <c r="AO83" s="87"/>
-      <c r="AP83" s="87"/>
-      <c r="AQ83" s="87"/>
-      <c r="AR83" s="87"/>
-      <c r="AS83" s="87"/>
-      <c r="AT83" s="87"/>
-      <c r="AU83" s="87"/>
-      <c r="AV83" s="87"/>
-      <c r="AW83" s="87"/>
-      <c r="AX83" s="87"/>
-      <c r="AY83" s="87"/>
-      <c r="AZ83" s="87"/>
-      <c r="BA83" s="87"/>
-      <c r="BB83" s="87"/>
-      <c r="BC83" s="87"/>
-      <c r="BD83" s="87"/>
-      <c r="BE83" s="87"/>
-      <c r="BF83" s="87"/>
-      <c r="BG83" s="87"/>
-      <c r="BH83" s="87"/>
-      <c r="BI83" s="87"/>
-      <c r="BJ83" s="87"/>
-      <c r="BK83" s="87"/>
-      <c r="BL83" s="86"/>
-      <c r="BM83" s="85"/>
-      <c r="BN83" s="86"/>
-      <c r="BO83" s="86"/>
-      <c r="BP83" s="87"/>
-      <c r="BQ83" s="87"/>
+      <c r="G83" s="91"/>
+      <c r="H83" s="91"/>
+      <c r="I83" s="84"/>
+      <c r="J83" s="84"/>
+      <c r="K83" s="85"/>
+      <c r="L83" s="85"/>
+      <c r="M83" s="86"/>
+      <c r="N83" s="86"/>
+      <c r="O83" s="86"/>
+      <c r="P83" s="86"/>
+      <c r="Q83" s="86"/>
+      <c r="R83" s="86"/>
+      <c r="S83" s="86"/>
+      <c r="T83" s="87"/>
+      <c r="U83" s="88"/>
+      <c r="V83" s="88"/>
+      <c r="W83" s="89"/>
+      <c r="X83" s="89"/>
+      <c r="Y83" s="86"/>
+      <c r="Z83" s="86"/>
+      <c r="AA83" s="86"/>
+      <c r="AB83" s="85"/>
+      <c r="AC83" s="85"/>
+      <c r="AD83" s="85"/>
+      <c r="AE83" s="85"/>
+      <c r="AF83" s="85"/>
+      <c r="AG83" s="85"/>
+      <c r="AH83" s="85"/>
+      <c r="AI83" s="85"/>
+      <c r="AJ83" s="85"/>
+      <c r="AK83" s="85"/>
+      <c r="AL83" s="85"/>
+      <c r="AM83" s="85"/>
+      <c r="AN83" s="85"/>
+      <c r="AO83" s="86"/>
+      <c r="AP83" s="86"/>
+      <c r="AQ83" s="86"/>
+      <c r="AR83" s="86"/>
+      <c r="AS83" s="86"/>
+      <c r="AT83" s="86"/>
+      <c r="AU83" s="86"/>
+      <c r="AV83" s="86"/>
+      <c r="AW83" s="86"/>
+      <c r="AX83" s="86"/>
+      <c r="AY83" s="86"/>
+      <c r="AZ83" s="86"/>
+      <c r="BA83" s="86"/>
+      <c r="BB83" s="86"/>
+      <c r="BC83" s="86"/>
+      <c r="BD83" s="86"/>
+      <c r="BE83" s="86"/>
+      <c r="BF83" s="86"/>
+      <c r="BG83" s="86"/>
+      <c r="BH83" s="86"/>
+      <c r="BI83" s="86"/>
+      <c r="BJ83" s="86"/>
+      <c r="BK83" s="86"/>
+      <c r="BL83" s="85"/>
+      <c r="BM83" s="84"/>
+      <c r="BN83" s="85"/>
+      <c r="BO83" s="85"/>
+      <c r="BP83" s="86"/>
+      <c r="BQ83" s="86"/>
       <c r="BR83" s="33"/>
       <c r="BS83" s="30"/>
       <c r="BT83" s="13"/>
@@ -9240,8 +9253,8 @@
       <c r="D85" s="49"/>
       <c r="E85" s="49"/>
       <c r="F85" s="19"/>
-      <c r="G85" s="83"/>
-      <c r="H85" s="83"/>
+      <c r="G85" s="82"/>
+      <c r="H85" s="82"/>
       <c r="I85" s="72"/>
       <c r="J85" s="27"/>
       <c r="K85" s="27"/>
@@ -9321,8 +9334,8 @@
       <c r="D86" s="49"/>
       <c r="E86" s="49"/>
       <c r="F86" s="70"/>
-      <c r="G86" s="84"/>
-      <c r="H86" s="84"/>
+      <c r="G86" s="83"/>
+      <c r="H86" s="83"/>
       <c r="I86" s="33"/>
       <c r="J86" s="33"/>
       <c r="K86" s="31"/>
@@ -9485,8 +9498,8 @@
       <c r="D88" s="49"/>
       <c r="E88" s="49"/>
       <c r="F88" s="72"/>
-      <c r="G88" s="83"/>
-      <c r="H88" s="83"/>
+      <c r="G88" s="82"/>
+      <c r="H88" s="82"/>
       <c r="I88" s="27"/>
       <c r="J88" s="27"/>
       <c r="K88" s="25"/>

</xml_diff>